<commit_message>
Added roster system with 6 specific positions (PG, SG, SF, PF, C, 6th Man)
</commit_message>
<xml_diff>
--- a/sportsref_download (3).xlsx
+++ b/sportsref_download (3).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ec4954651ec5d9f3/Documents/GitHub/nba-draft-app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iante\Downloads\NBA Draft App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{36587651-7288-47D4-A6A3-8BE0C12FF83E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC96006-069A-436A-BE2B-034B1566C928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10178" yWindow="0" windowWidth="10425" windowHeight="13043" xr2:uid="{B78C7215-33B7-4363-B67D-EB3EFE9C1878}"/>
+    <workbookView xWindow="2798" yWindow="3517" windowWidth="15389" windowHeight="9443" xr2:uid="{B78C7215-33B7-4363-B67D-EB3EFE9C1878}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -28,9 +28,6 @@
     <t>Player</t>
   </si>
   <si>
-    <t>TRB</t>
-  </si>
-  <si>
     <t>AST</t>
   </si>
   <si>
@@ -485,6 +482,9 @@
   </si>
   <si>
     <t>Donte DiVincenzo</t>
+  </si>
+  <si>
+    <t>REB</t>
   </si>
 </sst>
 </file>
@@ -1369,7 +1369,7 @@
   <dimension ref="A1:E151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1387,13 +1387,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
@@ -1401,7 +1401,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2">
         <v>32.700000000000003</v>
@@ -1418,7 +1418,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2">
         <v>30.4</v>
@@ -1435,7 +1435,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2">
         <v>29.6</v>
@@ -1452,7 +1452,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2">
         <v>28.2</v>
@@ -1469,7 +1469,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2">
         <v>27.6</v>
@@ -1486,7 +1486,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2">
         <v>26.8</v>
@@ -1503,7 +1503,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="2">
         <v>26.6</v>
@@ -1520,7 +1520,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2">
         <v>26.3</v>
@@ -1537,7 +1537,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2">
         <v>26.1</v>
@@ -1554,7 +1554,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="2">
         <v>26</v>
@@ -1571,7 +1571,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="2">
         <v>25.9</v>
@@ -1588,7 +1588,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="2">
         <v>25.6</v>
@@ -1605,7 +1605,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="2">
         <v>25.2</v>
@@ -1622,7 +1622,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="2">
         <v>24.9</v>
@@ -1639,7 +1639,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2">
         <v>24.7</v>
@@ -1656,7 +1656,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="2">
         <v>24.7</v>
@@ -1673,7 +1673,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="2">
         <v>24.6</v>
@@ -1690,7 +1690,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="2">
         <v>24.5</v>
@@ -1707,7 +1707,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="2">
         <v>24.4</v>
@@ -1724,7 +1724,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="2">
         <v>24.4</v>
@@ -1741,7 +1741,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="2">
         <v>24.3</v>
@@ -1758,7 +1758,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="2">
         <v>24.2</v>
@@ -1775,7 +1775,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="2">
         <v>24.2</v>
@@ -1792,7 +1792,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="2">
         <v>24</v>
@@ -1809,7 +1809,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" s="2">
         <v>24</v>
@@ -1826,7 +1826,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C27" s="2">
         <v>23.9</v>
@@ -1843,7 +1843,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" s="2">
         <v>23.8</v>
@@ -1860,7 +1860,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29" s="2">
         <v>23.5</v>
@@ -1877,7 +1877,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" s="2">
         <v>23.3</v>
@@ -1894,7 +1894,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C31" s="2">
         <v>23.2</v>
@@ -1911,7 +1911,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32" s="2">
         <v>22.8</v>
@@ -1928,7 +1928,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C33" s="2">
         <v>22.2</v>
@@ -1945,7 +1945,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C34" s="2">
         <v>22.2</v>
@@ -1962,7 +1962,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C35" s="2">
         <v>22.2</v>
@@ -1979,7 +1979,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C36" s="2">
         <v>22.2</v>
@@ -1996,7 +1996,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C37" s="2">
         <v>21.8</v>
@@ -2013,7 +2013,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C38" s="2">
         <v>21.6</v>
@@ -2030,7 +2030,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C39" s="2">
         <v>21.5</v>
@@ -2047,7 +2047,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C40" s="2">
         <v>21.4</v>
@@ -2064,7 +2064,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C41" s="2">
         <v>21.2</v>
@@ -2081,7 +2081,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C42" s="2">
         <v>21.1</v>
@@ -2098,7 +2098,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C43" s="2">
         <v>21.1</v>
@@ -2115,7 +2115,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C44" s="2">
         <v>21</v>
@@ -2132,7 +2132,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C45" s="2">
         <v>21</v>
@@ -2149,7 +2149,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C46" s="2">
         <v>20.6</v>
@@ -2166,7 +2166,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C47" s="2">
         <v>20.5</v>
@@ -2183,7 +2183,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C48" s="2">
         <v>20.399999999999999</v>
@@ -2200,7 +2200,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C49" s="2">
         <v>20.3</v>
@@ -2217,7 +2217,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C50" s="2">
         <v>20.2</v>
@@ -2234,7 +2234,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C51" s="2">
         <v>20.2</v>
@@ -2251,7 +2251,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C52" s="2">
         <v>19.5</v>
@@ -2268,7 +2268,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C53" s="2">
         <v>19.3</v>
@@ -2285,7 +2285,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C54" s="2">
         <v>19.3</v>
@@ -2302,7 +2302,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C55" s="2">
         <v>19.2</v>
@@ -2319,7 +2319,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C56" s="2">
         <v>19.100000000000001</v>
@@ -2336,7 +2336,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C57" s="2">
         <v>19.100000000000001</v>
@@ -2353,7 +2353,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C58" s="2">
         <v>19</v>
@@ -2370,7 +2370,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C59" s="2">
         <v>19</v>
@@ -2387,7 +2387,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C60" s="2">
         <v>18.899999999999999</v>
@@ -2404,7 +2404,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C61" s="2">
         <v>18.8</v>
@@ -2421,7 +2421,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C62" s="2">
         <v>18.7</v>
@@ -2438,7 +2438,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C63" s="2">
         <v>18.600000000000001</v>
@@ -2455,7 +2455,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C64" s="2">
         <v>18.5</v>
@@ -2472,7 +2472,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C65" s="2">
         <v>18.5</v>
@@ -2489,7 +2489,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C66" s="2">
         <v>18.5</v>
@@ -2506,7 +2506,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C67" s="2">
         <v>18.399999999999999</v>
@@ -2523,7 +2523,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C68" s="2">
         <v>18.2</v>
@@ -2540,7 +2540,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C69" s="2">
         <v>18.100000000000001</v>
@@ -2557,7 +2557,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C70" s="2">
         <v>18</v>
@@ -2574,7 +2574,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C71" s="2">
         <v>18</v>
@@ -2591,7 +2591,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C72" s="2">
         <v>17.600000000000001</v>
@@ -2608,7 +2608,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C73" s="2">
         <v>17.600000000000001</v>
@@ -2625,7 +2625,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C74" s="2">
         <v>17.5</v>
@@ -2642,7 +2642,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C75" s="2">
         <v>17.5</v>
@@ -2659,7 +2659,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C76" s="2">
         <v>17.2</v>
@@ -2676,7 +2676,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C77" s="2">
         <v>17.100000000000001</v>
@@ -2693,7 +2693,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C78" s="2">
         <v>17</v>
@@ -2710,7 +2710,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C79" s="2">
         <v>17</v>
@@ -2727,7 +2727,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C80" s="2">
         <v>16.899999999999999</v>
@@ -2744,7 +2744,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C81" s="2">
         <v>16.8</v>
@@ -2761,7 +2761,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C82" s="2">
         <v>16.8</v>
@@ -2778,7 +2778,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C83" s="2">
         <v>16.399999999999999</v>
@@ -2795,7 +2795,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C84" s="2">
         <v>16.3</v>
@@ -2812,7 +2812,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C85" s="2">
         <v>16.3</v>
@@ -2829,7 +2829,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C86" s="2">
         <v>16.2</v>
@@ -2846,7 +2846,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C87" s="2">
         <v>16.2</v>
@@ -2863,7 +2863,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C88" s="2">
         <v>16.2</v>
@@ -2880,7 +2880,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C89" s="2">
         <v>16.100000000000001</v>
@@ -2897,7 +2897,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C90" s="2">
         <v>15.6</v>
@@ -2914,7 +2914,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C91" s="2">
         <v>15.4</v>
@@ -2931,7 +2931,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C92" s="2">
         <v>15.3</v>
@@ -2948,7 +2948,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C93" s="2">
         <v>15.3</v>
@@ -2965,7 +2965,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C94" s="2">
         <v>15.3</v>
@@ -2982,7 +2982,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C95" s="2">
         <v>15.1</v>
@@ -2999,7 +2999,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C96" s="2">
         <v>15</v>
@@ -3016,7 +3016,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C97" s="2">
         <v>14.8</v>
@@ -3033,7 +3033,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C98" s="2">
         <v>14.7</v>
@@ -3050,7 +3050,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C99" s="2">
         <v>14.7</v>
@@ -3067,7 +3067,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C100" s="2">
         <v>14.7</v>
@@ -3084,7 +3084,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C101" s="2">
         <v>14.6</v>
@@ -3101,7 +3101,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C102" s="2">
         <v>14.6</v>
@@ -3118,7 +3118,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C103" s="2">
         <v>14.5</v>
@@ -3135,7 +3135,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C104" s="2">
         <v>14.4</v>
@@ -3152,7 +3152,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C105" s="2">
         <v>14.4</v>
@@ -3169,7 +3169,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C106" s="2">
         <v>14.4</v>
@@ -3186,7 +3186,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C107" s="2">
         <v>14.3</v>
@@ -3203,7 +3203,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C108" s="2">
         <v>14.2</v>
@@ -3220,7 +3220,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C109" s="2">
         <v>14.1</v>
@@ -3237,7 +3237,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C110" s="2">
         <v>14.1</v>
@@ -3254,7 +3254,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C111" s="2">
         <v>14.1</v>
@@ -3271,7 +3271,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C112" s="2">
         <v>14.1</v>
@@ -3288,7 +3288,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C113" s="2">
         <v>14</v>
@@ -3305,7 +3305,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C114" s="2">
         <v>14</v>
@@ -3322,7 +3322,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C115" s="2">
         <v>14</v>
@@ -3339,7 +3339,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C116" s="2">
         <v>13.9</v>
@@ -3356,7 +3356,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C117" s="2">
         <v>13.7</v>
@@ -3373,7 +3373,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C118" s="2">
         <v>13.6</v>
@@ -3390,7 +3390,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C119" s="2">
         <v>13.5</v>
@@ -3407,7 +3407,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C120" s="2">
         <v>13.4</v>
@@ -3424,7 +3424,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C121" s="2">
         <v>13.3</v>
@@ -3441,7 +3441,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C122" s="2">
         <v>13.2</v>
@@ -3458,7 +3458,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C123" s="2">
         <v>13.1</v>
@@ -3475,7 +3475,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C124" s="2">
         <v>13.1</v>
@@ -3492,7 +3492,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C125" s="2">
         <v>13</v>
@@ -3509,7 +3509,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C126" s="2">
         <v>13</v>
@@ -3526,7 +3526,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C127" s="2">
         <v>12.9</v>
@@ -3543,7 +3543,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C128" s="2">
         <v>12.7</v>
@@ -3560,7 +3560,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C129" s="2">
         <v>12.7</v>
@@ -3577,7 +3577,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C130" s="2">
         <v>12.7</v>
@@ -3594,7 +3594,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C131" s="2">
         <v>12.6</v>
@@ -3611,7 +3611,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C132" s="2">
         <v>12.6</v>
@@ -3628,7 +3628,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C133" s="2">
         <v>12.5</v>
@@ -3645,7 +3645,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C134" s="2">
         <v>12.5</v>
@@ -3662,7 +3662,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C135" s="2">
         <v>12.4</v>
@@ -3679,7 +3679,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C136" s="2">
         <v>12.4</v>
@@ -3696,7 +3696,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C137" s="2">
         <v>12.3</v>
@@ -3713,7 +3713,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C138" s="2">
         <v>12.3</v>
@@ -3730,7 +3730,7 @@
         <v>138</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C139" s="2">
         <v>12.3</v>
@@ -3747,7 +3747,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C140" s="2">
         <v>12.3</v>
@@ -3764,7 +3764,7 @@
         <v>140</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C141" s="2">
         <v>12.2</v>
@@ -3781,7 +3781,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C142" s="2">
         <v>12.2</v>
@@ -3798,7 +3798,7 @@
         <v>142</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C143" s="2">
         <v>12.1</v>
@@ -3815,7 +3815,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C144" s="2">
         <v>12.1</v>
@@ -3832,7 +3832,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C145" s="2">
         <v>12</v>
@@ -3849,7 +3849,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C146" s="2">
         <v>12</v>
@@ -3866,7 +3866,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C147" s="2">
         <v>12</v>
@@ -3883,7 +3883,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C148" s="2">
         <v>12</v>
@@ -3900,7 +3900,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C149" s="2">
         <v>11.9</v>
@@ -3917,7 +3917,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C150" s="2">
         <v>11.8</v>
@@ -3934,7 +3934,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C151" s="2">
         <v>11.7</v>

</xml_diff>

<commit_message>
Update project files with roster editing feature
</commit_message>
<xml_diff>
--- a/sportsref_download (3).xlsx
+++ b/sportsref_download (3).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iante\Downloads\NBA Draft App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC96006-069A-436A-BE2B-034B1566C928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1BC375-234C-4997-A88F-8507FDD67C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2798" yWindow="3517" windowWidth="15389" windowHeight="9443" xr2:uid="{B78C7215-33B7-4363-B67D-EB3EFE9C1878}"/>
+    <workbookView xWindow="300" yWindow="2835" windowWidth="15390" windowHeight="9443" xr2:uid="{B78C7215-33B7-4363-B67D-EB3EFE9C1878}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
   <si>
     <t>Rk</t>
   </si>
@@ -485,6 +485,9 @@
   </si>
   <si>
     <t>REB</t>
+  </si>
+  <si>
+    <t>Brandin Podziemski</t>
   </si>
 </sst>
 </file>
@@ -1366,15 +1369,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876D3B45-3B99-4C2A-A6C2-E5964AD0F784}">
-  <dimension ref="A1:E151"/>
+  <dimension ref="A1:E152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
+      <selection activeCell="A152" sqref="A152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.73046875" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="4.46484375" bestFit="1" customWidth="1"/>
   </cols>
@@ -3946,6 +3949,23 @@
         <v>3.6</v>
       </c>
     </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C152" s="2">
+        <v>11.7</v>
+      </c>
+      <c r="D152" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E152" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>